<commit_message>
Updated all the Test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/API_Data.xlsx
+++ b/src/test/resources/API_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samikshagupta\eclipse-workspace\ToDoList_Updated_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95BBC0B-1AF7-4A85-AA7B-670D53F40658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ED220E-F817-46F6-887B-5EFA1F2F303B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" tabRatio="779" activeTab="2" xr2:uid="{57D31B6C-5271-4BC7-9BCF-9A3C8BE0878B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>2021-09-15</t>
+  </si>
+  <si>
+    <t>monica.gellar@gmail.com</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2020-09-15</t>
   </si>
 </sst>
 </file>
@@ -175,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +203,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -208,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -217,6 +232,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -626,7 +644,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>123</v>
@@ -747,7 +765,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -767,31 +785,33 @@
     <hyperlink ref="F5" r:id="rId4" xr:uid="{A6B2D47D-7E56-4203-B1BC-6C9760C67AAA}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{6F2C8F60-AEE3-4866-AE6F-36FA91E0BBD2}"/>
     <hyperlink ref="C2" r:id="rId6" xr:uid="{C5F92072-28D0-4FA7-8493-2076D34896BD}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{647A60FC-71C6-4DFD-8279-AEB811B30E21}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{C437F271-641A-4A95-A9E5-009EABED098E}"/>
+    <hyperlink ref="C4" r:id="rId9" xr:uid="{756AB6B4-DDAB-4B94-AF75-0B93B1761553}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBE1EEA-4121-4765-8045-DAE84896E4D6}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.796875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="31.59765625" customWidth="1"/>
-    <col min="4" max="4" width="16.8984375" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -799,128 +819,85 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4">
+      <c r="D2" s="10">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3">
+        <v>123</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="E3">
+      <c r="D4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="4">
         <v>8</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>123</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>24</v>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{AFF9C6EE-9696-4F42-8290-BDDB19C98DF1}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{230D390A-CBAC-4CD3-887A-19B09B4A41BD}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{9010A4B3-2F9B-441F-A6DE-D925E31B9CFC}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{760AF226-B11D-4198-B89D-F40A8E1EC433}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{10203FC7-6649-412D-8BD1-D613FA8109A2}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{15A2284D-2B08-4E1E-8691-E89A41B783B0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>